<commit_message>
chnaged the dates to accurately reflect pay period cycles.
</commit_message>
<xml_diff>
--- a/data/hours_2_15_to_2_28.xlsx
+++ b/data/hours_2_15_to_2_28.xlsx
@@ -436,7 +436,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Person submitting this form:</t>
+          <t>Name</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -448,71 +448,71 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Larry Wallace Jr.</t>
+          <t>Antonio Montgomery</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>74</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Kiounis Williams</t>
+          <t>Azaniah Israel</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>20.25</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Antonio Montgomery</t>
+          <t>Cameron Morgan</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Cameron Morgan</t>
+          <t>Carlos Bautista</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Sonya Hosey</t>
+          <t>Felicia Chandler</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.75</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Kim Holiday</t>
+          <t>Jaqueline Oviedo</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.5</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Jaqueline Oviedo</t>
+          <t>Kim Holiday</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>38</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="9">
@@ -528,71 +528,71 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Larry Wallace Jr</t>
+          <t>Kiounis Williams</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>1</v>
+        <v>19.25</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Sonya Hosey</t>
+          <t>Larry Wallace Jr</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>2.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>The Bumgalows</t>
+          <t>Larry Wallace Jr.</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>2.5</v>
+        <v>74</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Viviana Varela</t>
+          <t>Sonya Hosey</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>20.25</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Azaniah Israel</t>
+          <t>Sonya Hosey</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>80</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Carlos Bautista</t>
+          <t>The Bumgalows</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>10</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Felicia Chandler</t>
+          <t>Viviana Varela</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>37</v>
+        <v>20.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>